<commit_message>
Retrieve camera format each time a camera is added or edited
</commit_message>
<xml_diff>
--- a/LocationsLoadFile.xlsx
+++ b/LocationsLoadFile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dpina\RiderProjects\cerberus-2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danipinartnadal/RiderProjects/cerberus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58BB3AE8-125D-459B-A043-E09049F14D97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1ED1CB5-708A-D24F-89C6-AEBA229D75CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -556,25 +556,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B6:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="B5" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="22.42578125" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" customWidth="1"/>
-    <col min="6" max="6" width="71.28515625" customWidth="1"/>
-    <col min="7" max="7" width="54.42578125" customWidth="1"/>
-    <col min="8" max="8" width="34.42578125" style="6" customWidth="1"/>
-    <col min="9" max="9" width="40.140625" customWidth="1"/>
-    <col min="10" max="10" width="44.140625" customWidth="1"/>
+    <col min="2" max="2" width="22.5" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" customWidth="1"/>
+    <col min="5" max="5" width="19.1640625" customWidth="1"/>
+    <col min="6" max="6" width="127.1640625" customWidth="1"/>
+    <col min="7" max="7" width="54.5" customWidth="1"/>
+    <col min="8" max="8" width="34.5" style="6" customWidth="1"/>
+    <col min="9" max="9" width="40.1640625" customWidth="1"/>
+    <col min="10" max="10" width="44.1640625" customWidth="1"/>
     <col min="11" max="11" width="48" customWidth="1"/>
-    <col min="12" max="12" width="45.7109375" customWidth="1"/>
+    <col min="12" max="12" width="45.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
@@ -603,7 +603,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>13</v>
       </c>
@@ -623,7 +623,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>13</v>
       </c>
@@ -640,7 +640,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>13</v>
       </c>
@@ -657,7 +657,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>15</v>
       </c>
@@ -674,7 +674,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>15</v>
       </c>
@@ -691,7 +691,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>15</v>
       </c>
@@ -708,7 +708,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
Feats/org struct/set camera format (#61)
* feat: implement dynamic hour height and scrollbar detection hooks for improved calendar layout

* refactor: simplify event conversion and integrate CalendarEvent type in SchedulerEvent

* Add postgres app to cerberus-dev

* Retrieve camera format each time a camera is added or edited

* feat: done

---------

Co-authored-by: Ángel Camuña <devluxe04@gmail.com>
</commit_message>
<xml_diff>
--- a/LocationsLoadFile.xlsx
+++ b/LocationsLoadFile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dpina\RiderProjects\cerberus-2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danipinartnadal/RiderProjects/cerberus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58BB3AE8-125D-459B-A043-E09049F14D97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1ED1CB5-708A-D24F-89C6-AEBA229D75CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -556,25 +556,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B6:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="B5" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="22.42578125" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" customWidth="1"/>
-    <col min="6" max="6" width="71.28515625" customWidth="1"/>
-    <col min="7" max="7" width="54.42578125" customWidth="1"/>
-    <col min="8" max="8" width="34.42578125" style="6" customWidth="1"/>
-    <col min="9" max="9" width="40.140625" customWidth="1"/>
-    <col min="10" max="10" width="44.140625" customWidth="1"/>
+    <col min="2" max="2" width="22.5" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" customWidth="1"/>
+    <col min="5" max="5" width="19.1640625" customWidth="1"/>
+    <col min="6" max="6" width="127.1640625" customWidth="1"/>
+    <col min="7" max="7" width="54.5" customWidth="1"/>
+    <col min="8" max="8" width="34.5" style="6" customWidth="1"/>
+    <col min="9" max="9" width="40.1640625" customWidth="1"/>
+    <col min="10" max="10" width="44.1640625" customWidth="1"/>
     <col min="11" max="11" width="48" customWidth="1"/>
-    <col min="12" max="12" width="45.7109375" customWidth="1"/>
+    <col min="12" max="12" width="45.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
@@ -603,7 +603,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>13</v>
       </c>
@@ -623,7 +623,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>13</v>
       </c>
@@ -640,7 +640,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>13</v>
       </c>
@@ -657,7 +657,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>15</v>
       </c>
@@ -674,7 +674,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>15</v>
       </c>
@@ -691,7 +691,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>15</v>
       </c>
@@ -708,7 +708,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>15</v>
       </c>

</xml_diff>